<commit_message>
1. Utworzono wersję tworzenia dat dla wariantu z liczbami arabskimi 2. Utworzono tworzenie insertów dla pliku z danymi dla firm 3. Wstępna normalizacja danych dla pliku z odpadami w mieście
</commit_message>
<xml_diff>
--- a/Data/Firmy.xlsx
+++ b/Data/Firmy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Zrodla\Harmonogram\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50636C27-E305-448A-88E8-E9586F30FFC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487A3E90-F65E-4FC1-BD62-CE43CE31970C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2760" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="49">
   <si>
     <t>ULICE</t>
   </si>
@@ -337,6 +337,9 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>Rodzaj odpadów</t>
   </si>
 </sst>
 </file>
@@ -988,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D0505D-1116-4CE1-9A43-A799B3F71EDF}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1030,9 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C2" s="13" t="s">
         <v>36</v>
       </c>

</xml_diff>